<commit_message>
Update SHACL Export-proct Activity
</commit_message>
<xml_diff>
--- a/Subtask5/03-eli-dl-ap-ep-activities/04-SHACL/EXPORT-PROC-Shapes.xlsx
+++ b/Subtask5/03-eli-dl-ap-ep-activities/04-SHACL/EXPORT-PROC-Shapes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
   <si>
     <t>Shapes URI</t>
   </si>
@@ -361,15 +361,9 @@
     <t>http://data.europarl.europa.eu/resource/eli/dl/iEpRegl/.*$/.*$</t>
   </si>
   <si>
-    <t>http://data.europarl.europa.eu/resource/eli/dl/proc/.*$</t>
-  </si>
-  <si>
     <t>eli-dl:LegislativeActivity</t>
   </si>
   <si>
-    <t>http://data.europarl.europa.eu/resource/eli/dl/proc/.*$/event/procedure-creation_1</t>
-  </si>
-  <si>
     <t>rdfs:Literal</t>
   </si>
   <si>
@@ -398,6 +392,102 @@
   </si>
   <si>
     <t>eli-dl:legislative_process_title</t>
+  </si>
+  <si>
+    <t>eli-dl:latest_activity</t>
+  </si>
+  <si>
+    <t>elidl-ep:hasActivityParticipation</t>
+  </si>
+  <si>
+    <t>eli-dl:consists_of</t>
+  </si>
+  <si>
+    <t>Constraints on LegislativeActivities</t>
+  </si>
+  <si>
+    <t>elidl-ep:activityType</t>
+  </si>
+  <si>
+    <t>eli-dl:activity_date</t>
+  </si>
+  <si>
+    <t>elidl-ep:activityId</t>
+  </si>
+  <si>
+    <t>elidl-ep:activityContextPrecision</t>
+  </si>
+  <si>
+    <t>elidl-ep:activityNature</t>
+  </si>
+  <si>
+    <t>eli-dl:occured_at_stage</t>
+  </si>
+  <si>
+    <t>elidl-ep:activityStatus</t>
+  </si>
+  <si>
+    <t>elidl-ep:amendmentDeadlineDate</t>
+  </si>
+  <si>
+    <t>eli-dl:hasActivityParticipation</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/activity-type/.*$</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/activity-context-precision/.*$</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/nature/.*$</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/activity-stage/[0-9][0-9]-[0-9][0-9]</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/activity-status/.*$</t>
+  </si>
+  <si>
+    <t>elidl-ep:ActivityParticipation</t>
+  </si>
+  <si>
+    <t>epsh:ActivityParticipation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>"^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>http://data.europarl.europa.eu/resource/eli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/dl/proc/[0-9][0-9][0-9][0-9]/[0-9a-zA-Z]*/[0-9a-zA-Z]*$"</t>
+    </r>
+  </si>
+  <si>
+    <t>"^http://data.europarl.europa.eu/resource/eli/dl/proc/[0-9][0-9][0-9][0-9]/[0-9][0-9][0-9][0-9]/[0-9a-zA-Z]*/event/[0-9a-zA-Z]*/main-dossier_[0-9]*/activity-participation_[0-9]*"</t>
+  </si>
+  <si>
+    <t>Constraints on ActivityParticipation</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1035,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="12.5" x14ac:dyDescent="0.5"/>
@@ -957,7 +1047,7 @@
     <col min="5" max="6" width="23.6796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.1328125" customWidth="1"/>
     <col min="8" max="8" width="19.31640625" customWidth="1"/>
-    <col min="9" max="9" width="53.04296875" customWidth="1"/>
+    <col min="9" max="9" width="81" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.6796875" customWidth="1"/>
     <col min="11" max="11" width="24.54296875" customWidth="1"/>
   </cols>
@@ -967,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
@@ -988,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>79</v>
@@ -1014,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>80</v>
@@ -1027,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>81</v>
@@ -1040,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1178,8 +1268,8 @@
       <c r="H15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>113</v>
+      <c r="I15" t="s">
+        <v>144</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>31</v>
@@ -1190,13 +1280,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
@@ -1205,9 +1295,6 @@
       <c r="H16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="J16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1215,14 +1302,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="13"/>
+      <c r="H17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>145</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="C18" s="14"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1230,33 +1333,33 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="13"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="13"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="3:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G25" s="1"/>
     </row>
   </sheetData>
@@ -1269,9 +1372,9 @@
     <hyperlink ref="C4" r:id="rId6"/>
     <hyperlink ref="C5" r:id="rId7"/>
     <hyperlink ref="C6" r:id="rId8"/>
-    <hyperlink ref="I15" r:id="rId9"/>
-    <hyperlink ref="I16" r:id="rId10"/>
-    <hyperlink ref="C7" r:id="rId11" display="http://data.europa.eu/eli/eli-draft-legislation-ontology"/>
+    <hyperlink ref="C7" r:id="rId9" display="http://data.europa.eu/eli/eli-draft-legislation-ontology"/>
+    <hyperlink ref="I15" r:id="rId10" display="http://data.europarl.europa.eu/resource/eli"/>
+    <hyperlink ref="I17" r:id="rId11" display="http://data.europarl.europa.eu/resource/eli/dl/proc/[0-9][0-9][0-9][0-9]/[0-9a-zA-Z]*/[0-9a-zA-Z]*/.*$"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -1284,11 +1387,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6796875" defaultRowHeight="12.5" x14ac:dyDescent="0.5"/>
@@ -1318,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
@@ -1340,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>79</v>
@@ -1366,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>80</v>
@@ -1379,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>81</v>
@@ -1392,10 +1495,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2"/>
       <c r="Q7" s="1"/>
@@ -1571,7 +1674,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:A27" si="0">CONCATENATE("epsh:P",ROW(A14))</f>
+        <f t="shared" ref="A14:A29" si="0">CONCATENATE("epsh:P",ROW(A14))</f>
         <v>epsh:P14</v>
       </c>
       <c r="B14" t="s">
@@ -1919,7 +2022,7 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
         <v>77</v>
@@ -1928,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G26" s="1">
         <v>1</v>
@@ -1943,8 +2046,324 @@
         <v>31</v>
       </c>
       <c r="T26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="1">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
         <v>117</v>
       </c>
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="1" t="str">
+        <f t="shared" ref="N29" si="1">LEFT(M29,1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="T33" s="19"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A44" si="2">CONCATENATE("epsh:P",ROW(A34))</f>
+        <v>epsh:P34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>30</v>
+      </c>
+      <c r="R34" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A35" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
+        <v>74</v>
+      </c>
+      <c r="M35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A36" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A37" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A38" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R38" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A39" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>30</v>
+      </c>
+      <c r="R39" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A40" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>30</v>
+      </c>
+      <c r="R40" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A41" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L41" t="s">
+        <v>30</v>
+      </c>
+      <c r="R41" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A42" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
+        <v>74</v>
+      </c>
+      <c r="M42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A43" t="str">
+        <f t="shared" si="2"/>
+        <v>epsh:P43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="T46" s="19"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A47" t="str">
+        <f t="shared" ref="A47" si="3">CONCATENATE("epsh:P",ROW(A47))</f>
+        <v>epsh:P47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C52"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1962,9 +2381,14 @@
     <hyperlink ref="R24" r:id="rId12"/>
     <hyperlink ref="R25" r:id="rId13"/>
     <hyperlink ref="C7" r:id="rId14" display="http://data.europa.eu/eli/eli-draft-legislation-ontology"/>
+    <hyperlink ref="R34" r:id="rId15"/>
+    <hyperlink ref="R38" r:id="rId16"/>
+    <hyperlink ref="R39" r:id="rId17"/>
+    <hyperlink ref="R40" r:id="rId18"/>
+    <hyperlink ref="R41" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>